<commit_message>
bugs fix like purchase info and product csv uplaod
</commit_message>
<xml_diff>
--- a/public/sample/Crops.xlsx
+++ b/public/sample/Crops.xlsx
@@ -1,31 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itsam\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA83E91-1106-47F5-AF38-F9810C2E1E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF561115-A260-48CA-B842-47906CC3B504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="21624" windowHeight="11124" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1416" yWindow="1116" windowWidth="21624" windowHeight="11124" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>CropName</t>
   </si>
@@ -33,13 +28,31 @@
     <t>Variety</t>
   </si>
   <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>ProductDescription</t>
+  </si>
+  <si>
+    <t>Composition</t>
+  </si>
+  <si>
     <t>Measurement</t>
   </si>
   <si>
+    <t>MeasurementIn</t>
+  </si>
+  <si>
     <t>Selling Status</t>
   </si>
   <si>
-    <t>Type</t>
+    <t>Expiry Date</t>
   </si>
   <si>
     <t>Purchase Price</t>
@@ -54,26 +67,71 @@
     <t>Final Price</t>
   </si>
   <si>
+    <t>Wheat Seeds</t>
+  </si>
+  <si>
+    <t>Seed</t>
+  </si>
+  <si>
+    <t>High yielding</t>
+  </si>
+  <si>
+    <t>Seeds</t>
+  </si>
+  <si>
+    <t>Kg</t>
+  </si>
+  <si>
+    <t>Available</t>
+  </si>
+  <si>
+    <t>2025-12-31</t>
+  </si>
+  <si>
+    <t>Rice Seeds</t>
+  </si>
+  <si>
+    <t>Resistant to pests</t>
+  </si>
+  <si>
+    <t>Kufri Badshah</t>
+  </si>
+  <si>
     <t>Potato</t>
   </si>
   <si>
-    <t>Kufri Jyoti</t>
-  </si>
-  <si>
-    <t>KG</t>
-  </si>
-  <si>
-    <t>Offline</t>
-  </si>
-  <si>
-    <t>Crops</t>
+    <t>Party Name</t>
+  </si>
+  <si>
+    <t>Mobile No</t>
+  </si>
+  <si>
+    <t>Company Name</t>
+  </si>
+  <si>
+    <t>Unit Price</t>
+  </si>
+  <si>
+    <t>Party GST</t>
+  </si>
+  <si>
+    <t>Company A</t>
+  </si>
+  <si>
+    <t>GST123</t>
+  </si>
+  <si>
+    <t>Company B</t>
+  </si>
+  <si>
+    <t>GST456</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,21 +140,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFCE9178"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FFCE9178"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF333333"/>
-      <name val="Verdana"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -108,7 +159,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -116,25 +167,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -157,44 +220,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -221,15 +284,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -256,7 +318,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -268,160 +329,184 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -433,49 +518,171 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2">
+        <v>500</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2">
-        <v>100</v>
-      </c>
-      <c r="G2">
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2">
+        <v>150</v>
+      </c>
+      <c r="M2">
+        <v>180</v>
+      </c>
+      <c r="N2">
+        <v>0.2</v>
+      </c>
+      <c r="O2">
+        <v>144</v>
+      </c>
+      <c r="Q2">
+        <v>1234567890</v>
+      </c>
+      <c r="R2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S2">
+        <v>10</v>
+      </c>
+      <c r="T2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <v>300</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3">
         <v>120</v>
       </c>
-      <c r="H2">
-        <v>7</v>
-      </c>
-      <c r="I2">
-        <v>1050</v>
+      <c r="M3">
+        <v>150</v>
+      </c>
+      <c r="N3">
+        <v>0.1</v>
+      </c>
+      <c r="O3">
+        <v>135</v>
+      </c>
+      <c r="Q3">
+        <v>9876543210</v>
+      </c>
+      <c r="R3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S3">
+        <v>25</v>
+      </c>
+      <c r="T3" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>